<commit_message>
Se termino de agragar la lista de la velocidad, se establecio el formato de mil separado por coma para ciertos resultados. Se corrigio un error en la lista de diametros ya que habia unos valores adicionales imnecesarios. Se creo la interpolacion para cuando la perdida del usuario coincide con la lista y los cfm no.
</commit_message>
<xml_diff>
--- a/datos/ValoresTabla/ListaValores.xlsx
+++ b/datos/ValoresTabla/ListaValores.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Android\Proy_Android_Studio\DimDucto2\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Android\Proy_Android_Studio\HVACTOOLS_v2\datos\ValoresTabla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BC38A44-25EE-43F3-ACDC-FC716A37D97A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B3C3D2-3E1C-46C5-9E58-B483DC99CECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21480" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DAF68F5B-3AC7-4AF7-8647-90CC53AC0645}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{DAF68F5B-3AC7-4AF7-8647-90CC53AC0645}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -176,21 +176,6 @@
   <dxfs count="4">
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -207,6 +192,21 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -262,8 +262,8 @@
     <tableColumn id="5" xr3:uid="{C9F92167-6BD7-47B8-A653-34C4FE8B3691}" name="Columna5">
       <calculatedColumnFormula>F2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{1E68C191-494E-453B-BB33-24713E293747}" name="Columna6" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{EE87BCC8-F6C6-4AC0-BD3C-D2874FD947A1}" name="Columna7" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{1E68C191-494E-453B-BB33-24713E293747}" name="Columna6" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{EE87BCC8-F6C6-4AC0-BD3C-D2874FD947A1}" name="Columna7" dataDxfId="0">
       <calculatedColumnFormula>H2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -571,15 +571,15 @@
   <dimension ref="B1:H1108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B1088" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1096" sqref="E1096"/>
+      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="35.140625" customWidth="1"/>
+    <col min="2" max="2" width="44.28515625" customWidth="1"/>
     <col min="3" max="6" width="12" customWidth="1"/>
     <col min="7" max="7" width="12" style="9" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" customWidth="1"/>

</xml_diff>